<commit_message>
RITM0167688 - Capy FIN009 Migration in line to SAP Upgrade.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessica.lara\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49CDB10-DFE8-40D2-A98C-70EF927E6CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4BAB53-901E-48F4-A143-4F05A6D75FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -321,7 +321,7 @@
     <t>EmailTo_Support</t>
   </si>
   <si>
-    <t>https://launchpad.orica.net/fiori#Shell-home</t>
+    <t>https://launchpad-dt.orica.net/fiori#Shell-home</t>
   </si>
 </sst>
 </file>
@@ -1827,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2046,7 +2046,7 @@
         <v>56</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3142,7 +3142,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B35" r:id="rId1" location="Shell-home" xr:uid="{A48EC6F5-D942-4657-80E2-98E16C3AC1D1}"/>
+    <hyperlink ref="B35" r:id="rId1" location="Shell-home" xr:uid="{210C780A-CD48-4283-B2B1-D63E1B2D723C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ITM0167688 - Update code in line to SAP Upgrade.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessica.lara\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4BAB53-901E-48F4-A143-4F05A6D75FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49CDB10-DFE8-40D2-A98C-70EF927E6CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -321,7 +321,7 @@
     <t>EmailTo_Support</t>
   </si>
   <si>
-    <t>https://launchpad-dt.orica.net/fiori#Shell-home</t>
+    <t>https://launchpad.orica.net/fiori#Shell-home</t>
   </si>
 </sst>
 </file>
@@ -1827,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2046,7 +2046,7 @@
         <v>56</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3142,7 +3142,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B35" r:id="rId1" location="Shell-home" xr:uid="{210C780A-CD48-4283-B2B1-D63E1B2D723C}"/>
+    <hyperlink ref="B35" r:id="rId1" location="Shell-home" xr:uid="{A48EC6F5-D942-4657-80E2-98E16C3AC1D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Selector - (Sharepoint Button file name )
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessica.lara\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49CDB10-DFE8-40D2-A98C-70EF927E6CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7AFE4D-27B9-41AB-A1B7-9FED1C262204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -183,145 +183,145 @@
     <t>InputFileName</t>
   </si>
   <si>
+    <t>Input File Name on SharePoint</t>
+  </si>
+  <si>
+    <t>SharePoint_InputFolderName</t>
+  </si>
+  <si>
+    <t>Fin009_Input</t>
+  </si>
+  <si>
+    <t>NoOfRetry_Login</t>
+  </si>
+  <si>
+    <t>SharePoint_Url</t>
+  </si>
+  <si>
+    <t>https://orica.sharepoint.com/teams/collab_000792/Shared%20Documents/Forms/AllItems.aspx?ga=1&amp;id=%2Fteams%2Fcollab%5F000792%2FShared%20Documents%2FCAPYBARA%20Remit%20Details&amp;viewid=4b1093b6%2D6a24%2D4ae1%2D81e4%2D11fb0a34b1ea</t>
+  </si>
+  <si>
+    <t>SharePoint Url for Fin009 process</t>
+  </si>
+  <si>
+    <t>VerySmallDelay</t>
+  </si>
+  <si>
+    <t>SmallDelay</t>
+  </si>
+  <si>
+    <t>MediumDelay</t>
+  </si>
+  <si>
+    <t>LargeDelay</t>
+  </si>
+  <si>
+    <t>VeryLargeDelay</t>
+  </si>
+  <si>
+    <t>C:\Users\</t>
+  </si>
+  <si>
+    <t>DownloadDirectory</t>
+  </si>
+  <si>
+    <t>InputFileSheetName</t>
+  </si>
+  <si>
+    <t>AU &amp; EU</t>
+  </si>
+  <si>
+    <t>excel,msedge</t>
+  </si>
+  <si>
+    <t>Retry_ExtractLineItems</t>
+  </si>
+  <si>
+    <t>SAP_ModuleName</t>
+  </si>
+  <si>
+    <t>Bank Statement Postprocessing</t>
+  </si>
+  <si>
+    <t>SAP_FioriUrl</t>
+  </si>
+  <si>
+    <t>ProcessOwnerEmail</t>
+  </si>
+  <si>
+    <t>ProcessOwner</t>
+  </si>
+  <si>
+    <t>ProcessName</t>
+  </si>
+  <si>
+    <t>EmailMessage_Success</t>
+  </si>
+  <si>
+    <t>Bot Run for Capybara Fin009 was successful</t>
+  </si>
+  <si>
+    <t>EmailMessage_Failure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bot has been Terminated </t>
+  </si>
+  <si>
+    <t>EmailSubject_Success</t>
+  </si>
+  <si>
+    <t>Cabybara Fin009 - Bot Processed Successfully</t>
+  </si>
+  <si>
+    <t>EmailSubject_Failure</t>
+  </si>
+  <si>
+    <t>Cabybara Fin009 - Bot Termination</t>
+  </si>
+  <si>
+    <t>StorageBucket_EmailTemplate</t>
+  </si>
+  <si>
+    <t>EmailTemplates</t>
+  </si>
+  <si>
+    <t>SuccessEmailTemplate</t>
+  </si>
+  <si>
+    <t>Success Template.html</t>
+  </si>
+  <si>
+    <t>ErrorTemplateEmail</t>
+  </si>
+  <si>
+    <t>Error Template.html</t>
+  </si>
+  <si>
+    <t>Capybara_Fin009_Dispatcher</t>
+  </si>
+  <si>
+    <t>PostingDate</t>
+  </si>
+  <si>
+    <t>02.02.2023</t>
+  </si>
+  <si>
+    <t>EmailMessage_NoItemsinQueue</t>
+  </si>
+  <si>
+    <t>EmailSubject_NoItemsinQueue</t>
+  </si>
+  <si>
+    <t>No Items in Data Table to add to queue</t>
+  </si>
+  <si>
+    <t>EmailTo_Support</t>
+  </si>
+  <si>
+    <t>https://launchpad.orica.net/fiori#Shell-home</t>
+  </si>
+  <si>
     <t>Co Code House Bank Account ID</t>
-  </si>
-  <si>
-    <t>Input File Name on SharePoint</t>
-  </si>
-  <si>
-    <t>SharePoint_InputFolderName</t>
-  </si>
-  <si>
-    <t>Fin009_Input</t>
-  </si>
-  <si>
-    <t>NoOfRetry_Login</t>
-  </si>
-  <si>
-    <t>SharePoint_Url</t>
-  </si>
-  <si>
-    <t>https://orica.sharepoint.com/teams/collab_000792/Shared%20Documents/Forms/AllItems.aspx?ga=1&amp;id=%2Fteams%2Fcollab%5F000792%2FShared%20Documents%2FCAPYBARA%20Remit%20Details&amp;viewid=4b1093b6%2D6a24%2D4ae1%2D81e4%2D11fb0a34b1ea</t>
-  </si>
-  <si>
-    <t>SharePoint Url for Fin009 process</t>
-  </si>
-  <si>
-    <t>VerySmallDelay</t>
-  </si>
-  <si>
-    <t>SmallDelay</t>
-  </si>
-  <si>
-    <t>MediumDelay</t>
-  </si>
-  <si>
-    <t>LargeDelay</t>
-  </si>
-  <si>
-    <t>VeryLargeDelay</t>
-  </si>
-  <si>
-    <t>C:\Users\</t>
-  </si>
-  <si>
-    <t>DownloadDirectory</t>
-  </si>
-  <si>
-    <t>InputFileSheetName</t>
-  </si>
-  <si>
-    <t>AU &amp; EU</t>
-  </si>
-  <si>
-    <t>excel,msedge</t>
-  </si>
-  <si>
-    <t>Retry_ExtractLineItems</t>
-  </si>
-  <si>
-    <t>SAP_ModuleName</t>
-  </si>
-  <si>
-    <t>Bank Statement Postprocessing</t>
-  </si>
-  <si>
-    <t>SAP_FioriUrl</t>
-  </si>
-  <si>
-    <t>ProcessOwnerEmail</t>
-  </si>
-  <si>
-    <t>ProcessOwner</t>
-  </si>
-  <si>
-    <t>ProcessName</t>
-  </si>
-  <si>
-    <t>EmailMessage_Success</t>
-  </si>
-  <si>
-    <t>Bot Run for Capybara Fin009 was successful</t>
-  </si>
-  <si>
-    <t>EmailMessage_Failure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bot has been Terminated </t>
-  </si>
-  <si>
-    <t>EmailSubject_Success</t>
-  </si>
-  <si>
-    <t>Cabybara Fin009 - Bot Processed Successfully</t>
-  </si>
-  <si>
-    <t>EmailSubject_Failure</t>
-  </si>
-  <si>
-    <t>Cabybara Fin009 - Bot Termination</t>
-  </si>
-  <si>
-    <t>StorageBucket_EmailTemplate</t>
-  </si>
-  <si>
-    <t>EmailTemplates</t>
-  </si>
-  <si>
-    <t>SuccessEmailTemplate</t>
-  </si>
-  <si>
-    <t>Success Template.html</t>
-  </si>
-  <si>
-    <t>ErrorTemplateEmail</t>
-  </si>
-  <si>
-    <t>Error Template.html</t>
-  </si>
-  <si>
-    <t>Capybara_Fin009_Dispatcher</t>
-  </si>
-  <si>
-    <t>PostingDate</t>
-  </si>
-  <si>
-    <t>02.02.2023</t>
-  </si>
-  <si>
-    <t>EmailMessage_NoItemsinQueue</t>
-  </si>
-  <si>
-    <t>EmailSubject_NoItemsinQueue</t>
-  </si>
-  <si>
-    <t>No Items in Data Table to add to queue</t>
-  </si>
-  <si>
-    <t>EmailTo_Support</t>
-  </si>
-  <si>
-    <t>https://launchpad.orica.net/fiori#Shell-home</t>
   </si>
 </sst>
 </file>
@@ -824,7 +824,7 @@
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -1820,15 +1820,18 @@
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;10&amp;K000000 General</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2015,7 +2018,7 @@
         <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
         <v>49</v>
@@ -2026,24 +2029,24 @@
         <v>51</v>
       </c>
       <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" t="s">
         <v>52</v>
-      </c>
-      <c r="C21" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
         <v>54</v>
-      </c>
-      <c r="B22" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -2052,169 +2055,162 @@
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C26" t="s">
         <v>58</v>
-      </c>
-      <c r="C26" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
         <v>54</v>
-      </c>
-      <c r="B27" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A29" t="s">
         <v>67</v>
       </c>
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-    </row>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1"/>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A35" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+      <c r="B34" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>91</v>
+      <c r="B37" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38" s="7" t="s">
         <v>78</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="2" t="s">
         <v>80</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="8" t="s">
         <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A44" t="s">
         <v>89</v>
       </c>
-      <c r="B44" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A46" t="s">
+    </row>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" t="s">
         <v>92</v>
       </c>
-      <c r="B46" t="s">
+    </row>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A47" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+      <c r="B47" t="s">
+        <v>95</v>
+      </c>
+    </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1">
       <c r="A48" t="s">
         <v>94</v>
       </c>
-      <c r="B48" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A49" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="51" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="52" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="53" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="54" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="55" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="56" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="57" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="58" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="59" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="60" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="61" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="62" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="63" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="64" spans="1:1" ht="14.25" customHeight="1"/>
+    </row>
+    <row r="49" ht="14.25" customHeight="1"/>
+    <row r="50" ht="14.25" customHeight="1"/>
+    <row r="51" ht="14.25" customHeight="1"/>
+    <row r="52" ht="14.25" customHeight="1"/>
+    <row r="53" ht="14.25" customHeight="1"/>
+    <row r="54" ht="14.25" customHeight="1"/>
+    <row r="55" ht="14.25" customHeight="1"/>
+    <row r="56" ht="14.25" customHeight="1"/>
+    <row r="57" ht="14.25" customHeight="1"/>
+    <row r="58" ht="14.25" customHeight="1"/>
+    <row r="59" ht="14.25" customHeight="1"/>
+    <row r="60" ht="14.25" customHeight="1"/>
+    <row r="61" ht="14.25" customHeight="1"/>
+    <row r="62" ht="14.25" customHeight="1"/>
+    <row r="63" ht="14.25" customHeight="1"/>
+    <row r="64" ht="14.25" customHeight="1"/>
     <row r="65" ht="14.25" customHeight="1"/>
     <row r="66" ht="14.25" customHeight="1"/>
     <row r="67" ht="14.25" customHeight="1"/>
@@ -3138,13 +3134,15 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B35" r:id="rId1" location="Shell-home" xr:uid="{A48EC6F5-D942-4657-80E2-98E16C3AC1D1}"/>
+    <hyperlink ref="B34" r:id="rId1" location="Shell-home" xr:uid="{A48EC6F5-D942-4657-80E2-98E16C3AC1D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;10&amp;K000000 General</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3202,10 +3200,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>45</v>
@@ -3213,10 +3211,10 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>45</v>
@@ -3224,10 +3222,10 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>45</v>
@@ -3235,10 +3233,10 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>45</v>
@@ -3246,10 +3244,10 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>45</v>
@@ -3257,10 +3255,10 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>45</v>
@@ -3268,10 +3266,10 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>45</v>
@@ -3279,10 +3277,10 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>45</v>
@@ -4292,5 +4290,8 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;10&amp;K000000 General</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>